<commit_message>
added abspaths for files
</commit_message>
<xml_diff>
--- a/accounts.xlsx
+++ b/accounts.xlsx
@@ -1,31 +1,77 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apellun/PycharmProjects/raschyot_rzki_i_gibki/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE31FCDB-B60F-5845-99F8-8AA9023638F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+  <si>
+    <t>Название чертежа</t>
+  </si>
+  <si>
+    <t>Материал</t>
+  </si>
+  <si>
+    <t>Толщина детали</t>
+  </si>
+  <si>
+    <t>Площадь детали</t>
+  </si>
+  <si>
+    <t>Цена детали</t>
+  </si>
+  <si>
+    <t>Резка, м.п</t>
+  </si>
+  <si>
+    <t>Врезка, количество</t>
+  </si>
+  <si>
+    <t>Цена врезки</t>
+  </si>
+  <si>
+    <t>Цена, рез+врезка</t>
+  </si>
+  <si>
+    <t>Количетво деталей</t>
+  </si>
+  <si>
+    <t>Стоимость деталей</t>
+  </si>
+  <si>
+    <t>Количетво комплектов</t>
+  </si>
+  <si>
+    <t>Стоимость комплектов</t>
+  </si>
+  <si>
+    <t>Тестовый чертеж</t>
+  </si>
+  <si>
+    <t>ст3</t>
+  </si>
+  <si>
+    <t>нерж</t>
+  </si>
+  <si>
+    <t>алюминий</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,14 +134,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -142,7 +180,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -174,27 +212,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,24 +246,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -419,56 +421,229 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+    <row r="1" spans="1:14">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>0.01</v>
+      </c>
+      <c r="F2">
+        <v>11.53</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>42</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>107.06</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>107.06</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0.01</v>
+      </c>
+      <c r="F3">
+        <v>11.53</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>122</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>267.06</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>267.06</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0.01</v>
+      </c>
+      <c r="F4">
+        <v>11.53</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>42</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>107.06</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>107.06</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+      <c r="F5">
+        <v>11.53</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>32</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>87.06</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>87.06</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>